<commit_message>
chore: add role models
</commit_message>
<xml_diff>
--- a/Assets/ArtRes/Excel/MonsterInfo.xlsx
+++ b/Assets/ArtRes/Excel/MonsterInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -39,37 +39,31 @@
     <t>hp</t>
   </si>
   <si>
-    <t>atkOffst</t>
-  </si>
-  <si>
-    <t>Zombie/1</t>
-  </si>
-  <si>
-    <t>Animator/Zombie/MonsterNormal</t>
-  </si>
-  <si>
-    <t>Zombie/2</t>
-  </si>
-  <si>
-    <t>Animator/Zombie/MonsterClimb</t>
-  </si>
-  <si>
-    <t>Zombie/3</t>
-  </si>
-  <si>
-    <t>Animator/Zombie/MonsterLazy</t>
-  </si>
-  <si>
-    <t>Zombie/4</t>
-  </si>
-  <si>
-    <t>Animator/Zombie/MonsterFast</t>
-  </si>
-  <si>
-    <t>Zombie/5</t>
-  </si>
-  <si>
-    <t>Zombie/6</t>
+    <t>atkOffset</t>
+  </si>
+  <si>
+    <t>Monster/Z1</t>
+  </si>
+  <si>
+    <t>Animator/Monster/Aggresive</t>
+  </si>
+  <si>
+    <t>Monster/Z2</t>
+  </si>
+  <si>
+    <t>Animator/Monster/Broken</t>
+  </si>
+  <si>
+    <t>Monster/Z3</t>
+  </si>
+  <si>
+    <t>Animator/Monster/Calm</t>
+  </si>
+  <si>
+    <t>Monster/Z4</t>
+  </si>
+  <si>
+    <t>Animator/Monster/Crawl</t>
   </si>
 </sst>
 </file>
@@ -77,10 +71,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -94,6 +88,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -106,29 +107,84 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,7 +199,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,92 +231,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,25 +245,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,157 +425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,24 +436,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,10 +456,32 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -500,6 +498,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,24 +528,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,148 +541,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1047,17 +1041,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="9.375" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="27.875" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1129,7 +1122,7 @@
         <v>50</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1155,7 +1148,7 @@
         <v>60</v>
       </c>
       <c r="F4">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>10</v>
@@ -1178,10 +1171,10 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -1195,7 +1188,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1204,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -1221,10 +1214,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>5</v>

</xml_diff>